<commit_message>
sementara ini pake 'skematik_bismillah' (punya kelompok sebelah) dulu buat simulasi dan jawab pertanyaan, rangkaian original kita pending dulu aja perbaikannya
</commit_message>
<xml_diff>
--- a/Tubes_Jadwal Beban_Kelompok D5.xlsx
+++ b/Tubes_Jadwal Beban_Kelompok D5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itbdsti-my.sharepoint.com/personal/13222087_mahasiswa_itb_ac_id/Documents/Documents/Academic/Semester 6/EL3017/Modul 3/Tubes-STE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{25C2D193-2150-484D-89B1-DBFBD2122ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C598D8C-2714-4096-BC5E-53BEECFA1807}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{25C2D193-2150-484D-89B1-DBFBD2122ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C5601A7-E45C-4397-A622-EE1E6C794595}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Prioritas" sheetId="3" r:id="rId4"/>
     <sheet name="Publik &amp; Sosial" sheetId="4" r:id="rId5"/>
     <sheet name="Rekapitulasi" sheetId="5" r:id="rId6"/>
+    <sheet name="Load Flow" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="129">
   <si>
     <t>No.</t>
   </si>
@@ -245,13 +246,193 @@
   </si>
   <si>
     <t>Daya Total (MVA)</t>
+  </si>
+  <si>
+    <t>Sesi 1</t>
+  </si>
+  <si>
+    <t>V (pu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PLTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PLTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RT2</t>
+  </si>
+  <si>
+    <t>0.6154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mall-Hotel</t>
+  </si>
+  <si>
+    <t>0.6682</t>
+  </si>
+  <si>
+    <t>0.1147</t>
+  </si>
+  <si>
+    <t>0.0556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumah ibadah</t>
+  </si>
+  <si>
+    <t>0.7289</t>
+  </si>
+  <si>
+    <t>0.1572</t>
+  </si>
+  <si>
+    <t>0.0760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RS</t>
+  </si>
+  <si>
+    <t>0.6864</t>
+  </si>
+  <si>
+    <t>0.1214</t>
+  </si>
+  <si>
+    <t>0.0588</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pusat Server Data</t>
+  </si>
+  <si>
+    <t>0.0030</t>
+  </si>
+  <si>
+    <t>0.0015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kantor Lembaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Istana Negara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pangkalan Militer</t>
+  </si>
+  <si>
+    <t>0.6865</t>
+  </si>
+  <si>
+    <t>0.2739</t>
+  </si>
+  <si>
+    <t>0.1324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RT3</t>
+  </si>
+  <si>
+    <t>0.4968</t>
+  </si>
+  <si>
+    <t>0.2403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RT4</t>
+  </si>
+  <si>
+    <t>0.5691</t>
+  </si>
+  <si>
+    <t>0.1269</t>
+  </si>
+  <si>
+    <t>0.0614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RT5</t>
+  </si>
+  <si>
+    <t>0.5683</t>
+  </si>
+  <si>
+    <t>0.1262</t>
+  </si>
+  <si>
+    <t>0.0611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Industri kecil</t>
+  </si>
+  <si>
+    <t>0.6685</t>
+  </si>
+  <si>
+    <t>0.7571</t>
+  </si>
+  <si>
+    <t>0.3671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Industri sedang</t>
+  </si>
+  <si>
+    <t>0.6713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Industri besar</t>
+  </si>
+  <si>
+    <t>0.6688</t>
+  </si>
+  <si>
+    <t>0.5557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Resto-Toko</t>
+  </si>
+  <si>
+    <t>0.6684</t>
+  </si>
+  <si>
+    <t>0.5735</t>
+  </si>
+  <si>
+    <t>0.2779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  UKM</t>
+  </si>
+  <si>
+    <t>0.7456</t>
+  </si>
+  <si>
+    <t>0.3607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Univ - Sekolah</t>
+  </si>
+  <si>
+    <t>0.6745</t>
+  </si>
+  <si>
+    <t>0.1194</t>
+  </si>
+  <si>
+    <t>0.0578</t>
+  </si>
+  <si>
+    <t>P (MW)</t>
+  </si>
+  <si>
+    <t>Q (MVAR)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -289,6 +470,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -426,6 +613,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB939A63-E09E-421B-86FF-FAD66D293812}">
   <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B30" sqref="B30:E35"/>
     </sheetView>
   </sheetViews>
@@ -4749,7 +4938,9 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5404,7 +5595,9 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5984,7 +6177,9 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6785,4 +6980,428 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C165A378-7894-41E8-A2E1-A45443D53C45}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="28">
+        <v>282382</v>
+      </c>
+      <c r="F3" s="29">
+        <v>10681000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="28">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="28">
+        <v>55101</v>
+      </c>
+      <c r="E4" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="F4" s="29">
+        <v>-11720000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="28">
+        <v>11117</v>
+      </c>
+      <c r="D5" s="28">
+        <v>22402</v>
+      </c>
+      <c r="E5" s="28">
+        <v>12729</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="28">
+        <v>11290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="28">
+        <v>11493</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="28">
+        <v>11616</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="28">
+        <v>11616</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="28">
+        <v>11616</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="28">
+        <v>11616</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="28">
+        <v>11616</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="28">
+        <v>11619</v>
+      </c>
+      <c r="D13" s="28">
+        <v>10851</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="28">
+        <v>11842</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="28">
+        <v>11842</v>
+      </c>
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="28">
+        <v>11290</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="28">
+        <v>11288</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="28">
+        <v>57343</v>
+      </c>
+      <c r="F17" s="28">
+        <v>27780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="28">
+        <v>11289</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="28">
+        <v>11471</v>
+      </c>
+      <c r="F18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="28">
+        <v>11290</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="28">
+        <v>11290</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="28">
+        <v>11516</v>
+      </c>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>